<commit_message>
Modify compare workbooks script
</commit_message>
<xml_diff>
--- a/TestCases/Tabulate/TalismanTestData.xlsx
+++ b/TestCases/Tabulate/TalismanTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A90984-5BF9-49B2-8A53-DC1D6AE02F79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82495999-3DB2-46FB-B2E7-D697C05DCB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1776" yWindow="3396" windowWidth="19896" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sapphire" sheetId="1" r:id="rId1"/>
@@ -680,17 +680,17 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="53.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -707,7 +707,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -725,7 +725,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -737,7 +737,7 @@
       </c>
       <c r="F3" s="28"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -749,13 +749,13 @@
       </c>
       <c r="F4" s="28"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F5" s="28"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F6" s="28"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -771,7 +771,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="28"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>4</v>
       </c>
@@ -787,23 +787,23 @@
       <c r="E8" s="14"/>
       <c r="F8" s="28"/>
     </row>
-    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="9"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="16">
         <f>AVERAGE(A8:D8)</f>
         <v>4.25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F2:F8"/>
@@ -824,17 +824,17 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="53.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -851,7 +851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -869,7 +869,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="F3" s="28"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -893,13 +893,13 @@
       </c>
       <c r="F4" s="28"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F5" s="28"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F6" s="28"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -915,7 +915,7 @@
       <c r="E7" s="21"/>
       <c r="F7" s="28"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>4</v>
       </c>
@@ -931,22 +931,22 @@
       <c r="E8" s="19"/>
       <c r="F8" s="28"/>
     </row>
-    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="16">
         <f>AVERAGE(A8:D8)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F2:F8"/>
@@ -967,17 +967,17 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="53.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -994,7 +994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="F3" s="28"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1036,13 +1036,13 @@
       </c>
       <c r="F4" s="28"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F5" s="28"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F6" s="28"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -1058,7 +1058,7 @@
       <c r="E7" s="21"/>
       <c r="F7" s="28"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1074,22 +1074,22 @@
       <c r="E8" s="19"/>
       <c r="F8" s="28"/>
     </row>
-    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F9" s="28"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="16">
         <f>AVERAGE(A8:D8)</f>
         <v>4.25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F2:F9"/>
@@ -1109,12 +1109,12 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>5</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>12</v>
       </c>
@@ -1136,19 +1136,16 @@
         <v>34</v>
       </c>
       <c r="C2" s="27">
-        <f>Sapphire!A8</f>
         <v>4</v>
       </c>
       <c r="D2" s="27">
-        <f>Opal!A8</f>
         <v>4</v>
       </c>
       <c r="E2" s="27">
-        <f>Emerald!A8</f>
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>13</v>
       </c>
@@ -1156,19 +1153,16 @@
         <v>35</v>
       </c>
       <c r="C3" s="27">
-        <f>Sapphire!B8</f>
         <v>4</v>
       </c>
       <c r="D3" s="27">
-        <f>Opal!B8</f>
         <v>5</v>
       </c>
       <c r="E3" s="27">
-        <f>Emerald!B8</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>15</v>
       </c>
@@ -1176,19 +1170,16 @@
         <v>36</v>
       </c>
       <c r="C4" s="27">
-        <f>Sapphire!C8</f>
         <v>4</v>
       </c>
       <c r="D4" s="27">
-        <f>Opal!C8</f>
         <v>4</v>
       </c>
       <c r="E4" s="27">
-        <f>Emerald!C8</f>
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>14</v>
       </c>
@@ -1196,22 +1187,19 @@
         <v>37</v>
       </c>
       <c r="C5" s="27">
-        <f>Sapphire!D8</f>
         <v>5</v>
       </c>
       <c r="D5" s="27">
-        <f>Opal!D8</f>
         <v>3</v>
       </c>
       <c r="E5" s="27">
-        <f>Emerald!D8</f>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="25"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>18</v>
       </c>
@@ -1219,15 +1207,12 @@
         <v>38</v>
       </c>
       <c r="C7" s="27">
-        <f>Sapphire!B11</f>
         <v>4.25</v>
       </c>
       <c r="D7" s="27">
-        <f>Opal!B11</f>
         <v>4</v>
       </c>
       <c r="E7" s="27">
-        <f>Emerald!B11</f>
         <v>4.25</v>
       </c>
     </row>

</xml_diff>